<commit_message>
New JSON has been created with template data but many Rules are still failing. Need to debug
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7819C70-F9C6-470F-A9F3-BCA1A4C373A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E690213C-AE66-4F86-B3B0-6DDBFF415008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="630" windowWidth="28770" windowHeight="15570" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="137">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -214,9 +214,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>transformers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of transformers modeled in User RMR &gt; Baseline RMR </t>
   </si>
   <si>
@@ -253,25 +250,208 @@
     <t>User RMR transformer name is not in the Baseline RMR</t>
   </si>
   <si>
-    <t>DICT_LIST</t>
-  </si>
-  <si>
-    <t>context</t>
-  </si>
-  <si>
     <t>rmr_template</t>
   </si>
   <si>
     <t>Section</t>
   </si>
   <si>
-    <t>name:Transformer_1,Transformer_2, Transformer_3</t>
-  </si>
-  <si>
-    <t>name:Transformer_1,Transformer_2</t>
-  </si>
-  <si>
-    <t>name:Transformer_1,Transformer_4</t>
+    <t>json_template</t>
+  </si>
+  <si>
+    <t>transformers[0]</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>peak_load</t>
+  </si>
+  <si>
+    <t>Transformer_1</t>
+  </si>
+  <si>
+    <t>transformers[1]</t>
+  </si>
+  <si>
+    <t>transformers[2]</t>
+  </si>
+  <si>
+    <t>Transformer_2</t>
+  </si>
+  <si>
+    <t>Transformer_3</t>
+  </si>
+  <si>
+    <t>Transformer_4</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Dry Single-Phase transformer modeled in the User Model whose efficiency is &gt; than Table 8.4.4. Baseline RMR equals Table 8.4.4</t>
+  </si>
+  <si>
+    <t>Dry Single-Phase transformer modeled in the User Model whose efficiency is &gt; than Table 8.4.4. Baseline RMR does not equal Table 8.4.4</t>
+  </si>
+  <si>
+    <t>Dry Three-Phase transformer modeled in the User Model whose efficiency is &gt; than Table 8.4.4. Baseline RMR matches Table 8.4.4</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>DRY_TYPE</t>
+  </si>
+  <si>
+    <t>SINGLE_PHASE</t>
+  </si>
+  <si>
+    <t>THREE_PHASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry Single-Phase transformer modeled in the User Model whose efficiency equals Table 8.4.4. </t>
+  </si>
+  <si>
+    <t>Dry Single-Phase transformer modeled in the User Model whose efficiency &lt; Table 8.4.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry Three-Phase transformer modeled in the User Model whose efficiency equals Table 8.4.4. </t>
+  </si>
+  <si>
+    <t>Dry Three-Phase transformer modeled in the User Model whose efficiency is &lt; than Table 8.4.4.</t>
+  </si>
+  <si>
+    <t>FLUID_FILLED</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Fluid-filled transformer modeled in the User Model, Baseline RMR equals User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Fluid-filled transformer modeled in the User Model, Baseline RMR does not equal User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, single phase transformer modeled in the User Model, Baseline RMR equals User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, single phase transformer modeled in the User Model, Baseline RMR does not equal User RMR</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Fluid-filled transformer modeled in the User Model, Proposed RMR equals User  RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Fluid-filled transformer modeled in the User Model, Proposed RMR doesn't equal User Model RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, single phase transformer modeled in the User Model, Proposed RMR equals User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, single phase transformer modeled in the User Model, Proposed RMR does not equal User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, three phase transformer modeled in the User Model, Proposed RMR equals User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, three phase transformer modeled in the User Model, Proposed RMR does not match User RMR</t>
+  </si>
+  <si>
+    <t>Transformer modeled in user RMR, Dry-type, three phase transformer modeled in the User Model, Proposed RMR efficiency matches User RMR but phase  does not match User RMR</t>
+  </si>
+  <si>
+    <t>rule-15-2a</t>
+  </si>
+  <si>
+    <t>rule-15-2b</t>
+  </si>
+  <si>
+    <t>rule-15-2c</t>
+  </si>
+  <si>
+    <t>rule-15-3a</t>
+  </si>
+  <si>
+    <t>rule-15-3b</t>
+  </si>
+  <si>
+    <t>rule-15-4a</t>
+  </si>
+  <si>
+    <t>rule-15-4b</t>
+  </si>
+  <si>
+    <t>rule-15-5a</t>
+  </si>
+  <si>
+    <t>rule-15-5b</t>
+  </si>
+  <si>
+    <t>rule-15-5c</t>
+  </si>
+  <si>
+    <t>rule-15-5d</t>
+  </si>
+  <si>
+    <t>rule-15-6a</t>
+  </si>
+  <si>
+    <t>rule-15-6b</t>
+  </si>
+  <si>
+    <t>rule-15-6c</t>
+  </si>
+  <si>
+    <t>rule-15-6d</t>
+  </si>
+  <si>
+    <t>rule-15-7a</t>
+  </si>
+  <si>
+    <t>rule-15-7b</t>
+  </si>
+  <si>
+    <t>rule-15-7c</t>
+  </si>
+  <si>
+    <t>rule-15-7d</t>
+  </si>
+  <si>
+    <t>rule-15-8a</t>
+  </si>
+  <si>
+    <t>rule-15-8b</t>
+  </si>
+  <si>
+    <t>rule-15-8c</t>
+  </si>
+  <si>
+    <t>rule-15-8d</t>
+  </si>
+  <si>
+    <t>rule-15-8e</t>
+  </si>
+  <si>
+    <t>rule-15-8f</t>
+  </si>
+  <si>
+    <t>rule-15-8g</t>
   </si>
 </sst>
 </file>
@@ -341,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -370,15 +550,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color theme="6" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="dashed">
         <color theme="6" tint="-0.24994659260841701"/>
@@ -402,11 +573,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right style="dashed">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -438,16 +651,237 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -779,30 +1213,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="52.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="33" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -813,52 +1247,102 @@
         <v>51</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="5" t="str">
         <f>"rule-"&amp;E2&amp;"-"&amp;E3&amp;E4</f>
         <v>rule-15-1a</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f t="shared" ref="F1:J1" si="0">"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
+        <f t="shared" ref="F1:G1" si="0">"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
         <v>rule-15-1b</v>
       </c>
       <c r="G1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-1c</v>
       </c>
-      <c r="H1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-15-2a</v>
-      </c>
-      <c r="I1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-15-2b</v>
-      </c>
-      <c r="J1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-15-2c</v>
-      </c>
-      <c r="K1" s="5" t="str">
-        <f t="shared" ref="K1:L1" si="1">"rule-"&amp;K2&amp;"-"&amp;K3&amp;K4</f>
-        <v>rule-15-3a</v>
-      </c>
-      <c r="L1" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>rule-15-3b</v>
-      </c>
-      <c r="M1" s="5" t="str">
-        <f t="shared" ref="M1:N1" si="2">"rule-"&amp;M2&amp;"-"&amp;M3&amp;M4</f>
-        <v>rule-15-4a</v>
-      </c>
-      <c r="N1" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>rule-15-4b</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -893,8 +1377,67 @@
       <c r="N2" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="3">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>15</v>
+      </c>
+      <c r="R2" s="3">
+        <v>15</v>
+      </c>
+      <c r="S2" s="3">
+        <v>15</v>
+      </c>
+      <c r="T2" s="3">
+        <v>15</v>
+      </c>
+      <c r="U2" s="3">
+        <v>15</v>
+      </c>
+      <c r="V2" s="3">
+        <v>15</v>
+      </c>
+      <c r="W2" s="3">
+        <v>15</v>
+      </c>
+      <c r="X2" s="3">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>15</v>
+      </c>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
@@ -931,8 +1474,67 @@
       <c r="N3" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="3">
+        <v>5</v>
+      </c>
+      <c r="P3" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>5</v>
+      </c>
+      <c r="R3" s="3">
+        <v>5</v>
+      </c>
+      <c r="S3" s="3">
+        <v>6</v>
+      </c>
+      <c r="T3" s="3">
+        <v>6</v>
+      </c>
+      <c r="U3" s="3">
+        <v>6</v>
+      </c>
+      <c r="V3" s="3">
+        <v>6</v>
+      </c>
+      <c r="W3" s="3">
+        <v>7</v>
+      </c>
+      <c r="X3" s="3">
+        <v>7</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>7</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>8</v>
+      </c>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+    </row>
+    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>55</v>
       </c>
@@ -969,8 +1571,67 @@
       <c r="N4" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="O4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+    </row>
+    <row r="5" spans="1:35" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -981,446 +1642,1697 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="M5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+    </row>
+    <row r="7" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="X7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="X9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="22"/>
+      <c r="AC9" s="22"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="22"/>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="C10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="O13" s="3">
+        <v>25</v>
+      </c>
+      <c r="P13" s="3">
+        <v>25</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>25</v>
+      </c>
+      <c r="R13" s="3">
+        <v>25</v>
+      </c>
+      <c r="W13" s="3">
+        <v>30</v>
+      </c>
+      <c r="X13" s="3">
+        <v>30</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>25</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>25</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>30</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>30</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>25</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>25</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>25</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>25</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22"/>
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22"/>
+    </row>
+    <row r="18" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="C18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L18" s="25"/>
+      <c r="M18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+    </row>
+    <row r="19" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="L20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG20" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="S21" s="3">
+        <v>25</v>
+      </c>
+      <c r="T21" s="3">
+        <v>25</v>
+      </c>
+      <c r="U21" s="3">
+        <v>25</v>
+      </c>
+      <c r="V21" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="V22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
+      <c r="V25" s="22"/>
+      <c r="W25" s="22"/>
+      <c r="X25" s="22"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="22"/>
+      <c r="AA25" s="22"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="22"/>
+      <c r="AD25" s="22"/>
+      <c r="AE25" s="22"/>
+      <c r="AF25" s="22"/>
+      <c r="AG25" s="22"/>
+    </row>
+    <row r="26" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
+      <c r="X26" s="25"/>
+      <c r="Y26" s="25"/>
+      <c r="Z26" s="25"/>
+      <c r="AA26" s="25"/>
+      <c r="AB26" s="25"/>
+      <c r="AC26" s="25"/>
+      <c r="AD26" s="25"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="25"/>
+      <c r="AG26" s="25"/>
+    </row>
+    <row r="27" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="25"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="25"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="AG28" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="AB30" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="AF30" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
+      <c r="V33" s="22"/>
+      <c r="W33" s="22"/>
+      <c r="X33" s="22"/>
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22"/>
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
+      <c r="AG33" s="22"/>
+    </row>
+    <row r="34" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="25"/>
+      <c r="W34" s="25"/>
+      <c r="X34" s="25"/>
+      <c r="Y34" s="25"/>
+      <c r="Z34" s="25"/>
+      <c r="AA34" s="25"/>
+      <c r="AB34" s="25"/>
+      <c r="AC34" s="25"/>
+      <c r="AD34" s="25"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="25"/>
+    </row>
+    <row r="35" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
+      <c r="S35" s="25"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="25"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="25"/>
+      <c r="X35" s="25"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="25"/>
+      <c r="AB35" s="25"/>
+      <c r="AC35" s="25"/>
+      <c r="AD35" s="25"/>
+      <c r="AE35" s="25"/>
+      <c r="AF35" s="25"/>
+      <c r="AG35" s="25"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J8" s="6" t="s">
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="O38" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="X38" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0.98299999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+      <c r="N41" s="22"/>
+      <c r="O41" s="22"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="22"/>
+      <c r="S41" s="22"/>
+      <c r="T41" s="22"/>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22"/>
+      <c r="W41" s="22"/>
+      <c r="X41" s="22"/>
+      <c r="Y41" s="22"/>
+      <c r="Z41" s="22"/>
+      <c r="AA41" s="22"/>
+      <c r="AB41" s="22"/>
+      <c r="AC41" s="22"/>
+      <c r="AD41" s="22"/>
+      <c r="AE41" s="22"/>
+      <c r="AF41" s="22"/>
+      <c r="AG41" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:D50 A5:D22">
-    <cfRule type="expression" dxfId="2" priority="6">
+  <conditionalFormatting sqref="A5:D6 C7:D9 A13:D14 A12:C12 A37:D40 D34 A34 A29:D33 D26 A26 A21:D25 D18 A18:B18 A16:D16 A10:D10">
+    <cfRule type="expression" dxfId="31" priority="70">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:D34 A35:B36">
-    <cfRule type="expression" dxfId="1" priority="5">
+  <conditionalFormatting sqref="A7:B9">
+    <cfRule type="expression" dxfId="30" priority="63">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:D36">
+  <conditionalFormatting sqref="A15:B15">
+    <cfRule type="expression" dxfId="29" priority="46">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:D13">
+    <cfRule type="expression" dxfId="28" priority="58">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:D21">
+    <cfRule type="expression" dxfId="27" priority="57">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="26" priority="44">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
+    <cfRule type="expression" dxfId="25" priority="34">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="expression" dxfId="24" priority="31">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="23" priority="48">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="22" priority="45">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="21" priority="41">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A17:B17">
+    <cfRule type="expression" dxfId="20" priority="49">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41 C41:D41">
+    <cfRule type="expression" dxfId="19" priority="35">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17 D19">
+    <cfRule type="expression" dxfId="18" priority="47">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11:B11">
+    <cfRule type="expression" dxfId="17" priority="33">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="16" priority="32">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="expression" dxfId="15" priority="21">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:D37">
+    <cfRule type="expression" dxfId="14" priority="38">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A19:B19">
+    <cfRule type="expression" dxfId="13" priority="28">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:C29">
+    <cfRule type="expression" dxfId="12" priority="40">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="expression" dxfId="11" priority="26">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D29">
+    <cfRule type="expression" dxfId="10" priority="23">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="9" priority="25">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:B27">
+    <cfRule type="expression" dxfId="8" priority="30">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35">
+    <cfRule type="expression" dxfId="7" priority="29">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="expression" dxfId="6" priority="27">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="expression" dxfId="5" priority="22">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="expression" dxfId="4" priority="18">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="expression" dxfId="2" priority="13">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E11:N11" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:N6" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
       <formula1>TEST_OUTCOME_TYPES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Made corrections to transformer JSON and spreadsheet
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E690213C-AE66-4F86-B3B0-6DDBFF415008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1491B-504A-4992-993C-7F7922ECBF4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="137">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -1216,8 +1216,8 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B42" sqref="B42"/>
+      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,13 +1839,9 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
-      <c r="L7" s="19" t="b">
-        <v>1</v>
-      </c>
+      <c r="L7" s="19"/>
       <c r="M7" s="19"/>
-      <c r="N7" s="19" t="b">
-        <v>1</v>
-      </c>
+      <c r="N7" s="19"/>
       <c r="O7" s="19" t="b">
         <v>1</v>
       </c>
@@ -1912,9 +1908,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4" t="b">
-        <v>1</v>
-      </c>
+      <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1969,9 +1963,7 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="22"/>
-      <c r="N9" s="22" t="b">
-        <v>1</v>
-      </c>
+      <c r="N9" s="22"/>
       <c r="O9" s="22" t="b">
         <v>1</v>
       </c>
@@ -2020,12 +2012,6 @@
       </c>
       <c r="D10" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>78</v>
@@ -2387,11 +2373,15 @@
       <c r="K18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L18" s="25"/>
+      <c r="L18" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="M18" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N18" s="25"/>
+      <c r="N18" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="O18" s="25"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="25"/>
@@ -2719,7 +2709,9 @@
       <c r="K26" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L26" s="25"/>
+      <c r="L26" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
       <c r="O26" s="25"/>
@@ -2959,7 +2951,9 @@
       <c r="M34" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N34" s="25"/>
+      <c r="N34" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="O34" s="25"/>
       <c r="P34" s="25"/>
       <c r="Q34" s="25"/>

</xml_diff>

<commit_message>
Fixed issues in the TCDs that caused issues in testing. Also fixed issues in Section 15 after running tests.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1491B-504A-4992-993C-7F7922ECBF4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F61B2F-0033-43FF-9ADC-139EBE1F9B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="138">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>rule-15-8g</t>
+  </si>
+  <si>
+    <t>Dry Three-Phase transformer modeled in the User Model whose efficiency is &gt; than Table 8.4.4. Baseline RMR does not match Table 8.4.4</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1219,8 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25"/>
+      <pane xSplit="4" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1681,7 @@
         <v>87</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>92</v>
@@ -2188,49 +2191,49 @@
         <v>76</v>
       </c>
       <c r="O13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="P13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="Q13" s="3">
-        <v>25</v>
+        <v>30000</v>
       </c>
       <c r="R13" s="3">
-        <v>25</v>
+        <v>30000</v>
       </c>
       <c r="W13" s="3">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="X13" s="3">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="Y13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="Z13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="AA13" s="3">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="AB13" s="3">
-        <v>30</v>
+        <v>30000</v>
       </c>
       <c r="AC13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="AD13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="AE13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="AF13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="AG13" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -2510,16 +2513,16 @@
         <v>76</v>
       </c>
       <c r="S21" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="T21" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="U21" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
       <c r="V21" s="3">
-        <v>25</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
@@ -3062,7 +3065,7 @@
         <v>0.98</v>
       </c>
       <c r="Q38" s="3">
-        <v>0.98299999999999998</v>
+        <v>0.98229999999999995</v>
       </c>
       <c r="R38" s="3">
         <v>0.98</v>

</xml_diff>

<commit_message>
Added units to transformer, lighting, and receptacle test spreadsheets and ruletest JSONs
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA27483-ACEF-42D6-963C-16C287FA2788}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94AAC10-D135-4B5F-8982-45E6264A9828}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="142">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -458,6 +458,15 @@
   </si>
   <si>
     <t>rmr_transformations</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>V*A</t>
   </si>
 </sst>
 </file>
@@ -495,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,8 +535,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -621,11 +636,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="6" tint="-0.24994659260841701"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -680,11 +732,870 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="69">
+  <dxfs count="190">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1478,11 +2389,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
-  <dimension ref="A1:AI53"/>
+  <dimension ref="A1:AJ78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AG10" sqref="AG10"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,17 +2404,18 @@
     <col min="2" max="2" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="52.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="33" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="52.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="34" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -1514,107 +2428,108 @@
       <c r="D1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="5" t="str">
-        <f>"rule-"&amp;E2&amp;"-"&amp;E3&amp;E4</f>
+      <c r="E1" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="5" t="str">
+        <f>"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
         <v>rule-15-1a</v>
       </c>
-      <c r="F1" s="5" t="str">
-        <f t="shared" ref="F1:G1" si="0">"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
+      <c r="G1" s="5" t="str">
+        <f t="shared" ref="G1:H1" si="0">"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
         <v>rule-15-1b</v>
       </c>
-      <c r="G1" s="5" t="str">
+      <c r="H1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-1c</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="3">
-        <v>15</v>
-      </c>
+      <c r="E2" s="27"/>
       <c r="F2" s="3">
         <v>15</v>
       </c>
@@ -1699,19 +2614,20 @@
       <c r="AG2" s="3">
         <v>15</v>
       </c>
-      <c r="AH2" s="3"/>
+      <c r="AH2" s="3">
+        <v>15</v>
+      </c>
       <c r="AI2" s="3"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="3"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
+      <c r="E3" s="27"/>
       <c r="F3" s="3">
         <v>1</v>
       </c>
@@ -1719,7 +2635,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="3">
         <v>2</v>
@@ -1728,19 +2644,19 @@
         <v>2</v>
       </c>
       <c r="K3" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="3">
         <v>3</v>
       </c>
       <c r="M3" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="3">
         <v>4</v>
       </c>
       <c r="O3" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P3" s="3">
         <v>5</v>
@@ -1752,7 +2668,7 @@
         <v>5</v>
       </c>
       <c r="S3" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T3" s="3">
         <v>6</v>
@@ -1764,7 +2680,7 @@
         <v>6</v>
       </c>
       <c r="W3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X3" s="3">
         <v>7</v>
@@ -1776,7 +2692,7 @@
         <v>7</v>
       </c>
       <c r="AA3" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB3" s="3">
         <v>8</v>
@@ -1796,299 +2712,305 @@
       <c r="AG3" s="3">
         <v>8</v>
       </c>
-      <c r="AH3" s="3"/>
+      <c r="AH3" s="3">
+        <v>8</v>
+      </c>
       <c r="AI3" s="3"/>
-    </row>
-    <row r="4" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ3" s="3"/>
+    </row>
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
-    </row>
-    <row r="5" spans="1:35" ht="60" x14ac:dyDescent="0.25">
+      <c r="AJ4" s="3"/>
+    </row>
+    <row r="5" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="U5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="V6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="W6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="Y6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Z6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="AA6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
-    </row>
-    <row r="7" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>68</v>
       </c>
@@ -2097,7 +3019,7 @@
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="19"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -2107,57 +3029,73 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
-      <c r="O7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="P7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="S7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Q7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="R7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="S7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="T7" s="19"/>
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
-      <c r="W7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="X7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W7" s="19"/>
+      <c r="X7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Y7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Z7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AA7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AB7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AC7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AD7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AE7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AF7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AG7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AH7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -2166,7 +3104,7 @@
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -2188,29 +3126,37 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
-      <c r="AA8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA8" s="4"/>
+      <c r="AB8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AC8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AD8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AE8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AF8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AG8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AH8" s="4" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>68</v>
       </c>
@@ -2219,53 +3165,62 @@
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
-      <c r="M9" s="22"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="22"/>
-      <c r="O9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="S9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Q9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="R9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="S9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="T9" s="22"/>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
-      <c r="W9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="X9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Y9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="Z9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AA9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="AB9" s="22"/>
       <c r="AC9" s="22"/>
       <c r="AD9" s="22"/>
       <c r="AE9" s="22"/>
       <c r="AF9" s="22"/>
       <c r="AG9" s="22"/>
-    </row>
-    <row r="10" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH9" s="22"/>
+    </row>
+    <row r="10" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>68</v>
       </c>
@@ -2278,20 +3233,17 @@
       <c r="D10" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="25"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="25" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
+      <c r="O10" s="25"/>
       <c r="P10" s="25" t="str">
         <f>"1"</f>
         <v>1</v>
@@ -2304,56 +3256,60 @@
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="S10" s="25"/>
+      <c r="S10" s="25" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
-      <c r="W10" s="25" t="str">
-        <f>"1"</f>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25" t="str">
+        <f t="shared" ref="X10:AH10" si="1">"1"</f>
         <v>1</v>
       </c>
-      <c r="X10" s="25" t="str">
-        <f>"1"</f>
+      <c r="Y10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Y10" s="25" t="str">
-        <f>"1"</f>
+      <c r="Z10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Z10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AA10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AA10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AB10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AB10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AC10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AC10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AD10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AE10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AE10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AF10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AF10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AG10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AG10" s="25" t="str">
-        <f>"1"</f>
+      <c r="AH10" s="25" t="str">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>68</v>
       </c>
@@ -2366,9 +3322,7 @@
       <c r="D11" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="E11" s="28"/>
       <c r="P11" s="3" t="s">
         <v>77</v>
       </c>
@@ -2378,7 +3332,7 @@
       <c r="R11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="W11" s="3" t="s">
+      <c r="S11" s="3" t="s">
         <v>77</v>
       </c>
       <c r="X11" s="3" t="s">
@@ -2411,8 +3365,11 @@
       <c r="AG11" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
@@ -2425,9 +3382,7 @@
       <c r="D12" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="E12" s="28"/>
       <c r="P12" s="3" t="s">
         <v>88</v>
       </c>
@@ -2437,26 +3392,26 @@
       <c r="R12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="W12" s="3" t="s">
-        <v>95</v>
+      <c r="S12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>88</v>
       </c>
       <c r="AA12" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AD12" s="3" t="s">
         <v>88</v>
@@ -2470,8 +3425,11 @@
       <c r="AG12" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH12" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>68</v>
       </c>
@@ -2484,41 +3442,39 @@
       <c r="D13" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="E13" s="28"/>
       <c r="P13" s="3" t="s">
         <v>89</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="W13" s="3" t="s">
+      <c r="S13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>89</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AB13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AC13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD13" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="AD13" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>90</v>
@@ -2526,8 +3482,11 @@
       <c r="AF13" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AG13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
@@ -2540,38 +3499,38 @@
       <c r="D14" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="O14" s="3">
-        <v>25000</v>
+      <c r="E14" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="P14" s="3">
         <v>25000</v>
       </c>
       <c r="Q14" s="3">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="R14" s="3">
         <v>30000</v>
       </c>
-      <c r="W14" s="3">
+      <c r="S14" s="3">
         <v>30000</v>
       </c>
       <c r="X14" s="3">
         <v>30000</v>
       </c>
       <c r="Y14" s="3">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="Z14" s="3">
         <v>25000</v>
       </c>
       <c r="AA14" s="3">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="AB14" s="3">
         <v>30000</v>
       </c>
       <c r="AC14" s="3">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="AD14" s="3">
         <v>25000</v>
@@ -2585,8 +3544,11 @@
       <c r="AG14" s="3">
         <v>25000</v>
       </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AH14" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>68</v>
       </c>
@@ -2599,29 +3561,30 @@
       <c r="D15" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="P15" s="3">
+      <c r="E15" s="28"/>
+      <c r="Q15" s="3">
         <v>0.99</v>
       </c>
-      <c r="W15" s="3">
+      <c r="X15" s="3">
         <v>0.98</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="Z15" s="3">
         <v>0.98</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="AB15" s="3">
         <v>0.98</v>
       </c>
-      <c r="AC15" s="3">
+      <c r="AD15" s="3">
         <v>0.99</v>
       </c>
-      <c r="AE15" s="3">
+      <c r="AF15" s="3">
         <v>0.99</v>
       </c>
-      <c r="AG15" s="3">
+      <c r="AH15" s="3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>68</v>
       </c>
@@ -2634,8 +3597,11 @@
       <c r="D16" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E16" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>68</v>
       </c>
@@ -2648,8 +3614,9 @@
       <c r="D17" s="12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>68</v>
       </c>
@@ -2662,8 +3629,9 @@
       <c r="D18" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E18" s="28"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>68</v>
       </c>
@@ -2676,8 +3644,9 @@
       <c r="D19" s="12" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>68</v>
       </c>
@@ -2690,7 +3659,7 @@
       <c r="D20" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
@@ -2719,8 +3688,9 @@
       <c r="AE20" s="22"/>
       <c r="AF20" s="22"/>
       <c r="AG20" s="22"/>
-    </row>
-    <row r="21" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH20" s="22"/>
+    </row>
+    <row r="21" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>138</v>
       </c>
@@ -2733,54 +3703,51 @@
       <c r="D21" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="25" t="str">
-        <f>"1"</f>
+      <c r="E21" s="28"/>
+      <c r="F21" s="25" t="str">
+        <f t="shared" ref="F21:O21" si="2">"1"</f>
         <v>1</v>
       </c>
-      <c r="F21" s="25" t="str">
-        <f>"1"</f>
+      <c r="G21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G21" s="25" t="str">
-        <f>"1"</f>
+      <c r="H21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H21" s="25" t="str">
-        <f>"1"</f>
+      <c r="I21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="I21" s="25" t="str">
-        <f>"1"</f>
+      <c r="J21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J21" s="25" t="str">
-        <f>"1"</f>
+      <c r="K21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K21" s="25" t="str">
-        <f>"1"</f>
+      <c r="L21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="L21" s="25" t="str">
-        <f>"1"</f>
+      <c r="M21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M21" s="25" t="str">
-        <f>"1"</f>
+      <c r="N21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N21" s="25" t="str">
-        <f>"1"</f>
+      <c r="O21" s="25" t="str">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O21" s="25"/>
       <c r="P21" s="25"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
-      <c r="S21" s="25" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
+      <c r="S21" s="25"/>
       <c r="T21" s="25" t="str">
         <f>"1"</f>
         <v>1</v>
@@ -2793,7 +3760,10 @@
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="W21" s="25"/>
+      <c r="W21" s="25" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="X21" s="25"/>
       <c r="Y21" s="25"/>
       <c r="Z21" s="25"/>
@@ -2804,8 +3774,9 @@
       <c r="AE21" s="25"/>
       <c r="AF21" s="25"/>
       <c r="AG21" s="25"/>
-    </row>
-    <row r="22" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH21" s="25"/>
+    </row>
+    <row r="22" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>138</v>
       </c>
@@ -2818,9 +3789,7 @@
       <c r="D22" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="E22" s="28"/>
       <c r="F22" s="3" t="s">
         <v>77</v>
       </c>
@@ -2848,13 +3817,13 @@
       <c r="N22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O22" s="25"/>
+      <c r="O22" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="P22" s="25"/>
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
-      <c r="S22" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="S22" s="25"/>
       <c r="T22" s="3" t="s">
         <v>77</v>
       </c>
@@ -2864,7 +3833,9 @@
       <c r="V22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="W22" s="3"/>
+      <c r="W22" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
@@ -2875,8 +3846,9 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
-    </row>
-    <row r="23" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH22" s="3"/>
+    </row>
+    <row r="23" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>138</v>
       </c>
@@ -2889,23 +3861,21 @@
       <c r="D23" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="28"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="25"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="3"/>
       <c r="O23" s="25"/>
       <c r="P23" s="25"/>
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
-      <c r="S23" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="S23" s="25"/>
       <c r="T23" s="3" t="s">
         <v>88</v>
       </c>
@@ -2915,7 +3885,9 @@
       <c r="V23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="W23" s="3"/>
+      <c r="W23" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
@@ -2926,8 +3898,9 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH23" s="3"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>138</v>
       </c>
@@ -2940,29 +3913,30 @@
       <c r="D24" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="N24" s="6"/>
+      <c r="E24" s="28"/>
+      <c r="M24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
-      <c r="S24" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="S24" s="6"/>
       <c r="T24" s="3" t="s">
         <v>89</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AG24" s="3" t="s">
+      <c r="W24" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH24" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>138</v>
       </c>
@@ -2975,8 +3949,8 @@
       <c r="D25" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="S25" s="3">
-        <v>25000</v>
+      <c r="E25" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="T25" s="3">
         <v>25000</v>
@@ -2987,8 +3961,11 @@
       <c r="V25" s="3">
         <v>25000</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="W25" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>138</v>
       </c>
@@ -3001,44 +3978,45 @@
       <c r="D26" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="O26" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="Q26" s="3">
+      <c r="E26" s="28"/>
+      <c r="P26" s="3">
         <v>0.99</v>
       </c>
       <c r="R26" s="3">
         <v>0.99</v>
       </c>
       <c r="S26" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="T26" s="3">
         <v>0.98</v>
       </c>
-      <c r="T26" s="3">
+      <c r="U26" s="3">
         <v>0.97</v>
       </c>
-      <c r="U26" s="3">
+      <c r="V26" s="3">
         <v>0.98299999999999998</v>
       </c>
-      <c r="V26" s="3">
+      <c r="W26" s="3">
         <v>0.98</v>
       </c>
-      <c r="X26" s="3">
+      <c r="Y26" s="3">
         <v>0.98</v>
       </c>
-      <c r="Z26" s="3">
+      <c r="AA26" s="3">
         <v>0.98</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AC26" s="3">
         <v>0.98</v>
       </c>
-      <c r="AD26" s="3">
+      <c r="AE26" s="3">
         <v>0.99</v>
       </c>
-      <c r="AF26" s="3">
+      <c r="AG26" s="3">
         <v>0.99</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>138</v>
       </c>
@@ -3051,8 +4029,11 @@
       <c r="D27" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E27" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>138</v>
       </c>
@@ -3065,9 +4046,7 @@
       <c r="D28" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E28" s="3">
-        <v>2</v>
-      </c>
+      <c r="E28" s="28"/>
       <c r="F28" s="3">
         <v>2</v>
       </c>
@@ -3095,8 +4074,11 @@
       <c r="N28" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="O28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>138</v>
       </c>
@@ -3109,9 +4091,7 @@
       <c r="D29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="E29" s="28"/>
       <c r="F29" s="3" t="s">
         <v>80</v>
       </c>
@@ -3139,8 +4119,11 @@
       <c r="N29" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="O29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>138</v>
       </c>
@@ -3153,20 +4136,21 @@
       <c r="D30" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="3">
-        <v>3</v>
-      </c>
+      <c r="E30" s="28"/>
       <c r="F30" s="3">
         <v>3</v>
       </c>
-      <c r="H30" s="3">
+      <c r="G30" s="3">
         <v>3</v>
       </c>
       <c r="I30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>138</v>
       </c>
@@ -3179,20 +4163,20 @@
       <c r="D31" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="22" t="s">
-        <v>81</v>
-      </c>
+      <c r="E31" s="30"/>
       <c r="F31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22" t="s">
+      <c r="G31" s="22" t="s">
         <v>81</v>
       </c>
+      <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="J31" s="22"/>
+      <c r="J31" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
@@ -3216,8 +4200,9 @@
       <c r="AE31" s="22"/>
       <c r="AF31" s="22"/>
       <c r="AG31" s="22"/>
-    </row>
-    <row r="32" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH31" s="22"/>
+    </row>
+    <row r="32" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>138</v>
       </c>
@@ -3230,12 +4215,10 @@
       <c r="D32" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E32" s="25"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
-      <c r="H32" s="25">
-        <v>1</v>
-      </c>
+      <c r="H32" s="25"/>
       <c r="I32" s="25">
         <v>1</v>
       </c>
@@ -3248,7 +4231,9 @@
       <c r="L32" s="25">
         <v>1</v>
       </c>
-      <c r="M32" s="25"/>
+      <c r="M32" s="25">
+        <v>1</v>
+      </c>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
@@ -3269,8 +4254,9 @@
       <c r="AE32" s="25"/>
       <c r="AF32" s="25"/>
       <c r="AG32" s="25"/>
-    </row>
-    <row r="33" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH32" s="25"/>
+    </row>
+    <row r="33" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>138</v>
       </c>
@@ -3283,12 +4269,10 @@
       <c r="D33" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="25"/>
+      <c r="E33" s="28"/>
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="H33" s="25"/>
       <c r="I33" s="3" t="s">
         <v>77</v>
       </c>
@@ -3301,7 +4285,9 @@
       <c r="L33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="25"/>
+      <c r="M33" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="N33" s="25"/>
       <c r="O33" s="25"/>
       <c r="P33" s="25"/>
@@ -3322,8 +4308,9 @@
       <c r="AE33" s="25"/>
       <c r="AF33" s="25"/>
       <c r="AG33" s="25"/>
-    </row>
-    <row r="34" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH33" s="25"/>
+    </row>
+    <row r="34" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>138</v>
       </c>
@@ -3336,14 +4323,14 @@
       <c r="D34" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="25"/>
+      <c r="E34" s="28"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="3"/>
+      <c r="H34" s="25"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="25"/>
+      <c r="L34" s="3"/>
       <c r="M34" s="25"/>
       <c r="N34" s="25"/>
       <c r="O34" s="25"/>
@@ -3365,8 +4352,9 @@
       <c r="AE34" s="25"/>
       <c r="AF34" s="25"/>
       <c r="AG34" s="25"/>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH34" s="25"/>
+    </row>
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>138</v>
       </c>
@@ -3379,11 +4367,12 @@
       <c r="D35" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AG35" s="3" t="s">
+      <c r="E35" s="28"/>
+      <c r="AH35" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>138</v>
       </c>
@@ -3396,8 +4385,11 @@
       <c r="D36" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E36" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>138</v>
       </c>
@@ -3410,17 +4402,18 @@
       <c r="D37" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AB37" s="3">
+      <c r="E37" s="28"/>
+      <c r="AC37" s="3">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AD37" s="3">
+      <c r="AE37" s="3">
         <v>0.98</v>
       </c>
-      <c r="AF37" s="3">
+      <c r="AG37" s="3">
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>138</v>
       </c>
@@ -3433,8 +4426,11 @@
       <c r="D38" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E38" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>138</v>
       </c>
@@ -3447,9 +4443,7 @@
       <c r="D39" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H39" s="3">
-        <v>2</v>
-      </c>
+      <c r="E39" s="28"/>
       <c r="I39" s="3">
         <v>2</v>
       </c>
@@ -3460,10 +4454,13 @@
         <v>2</v>
       </c>
       <c r="L39" s="3">
+        <v>2</v>
+      </c>
+      <c r="M39" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>138</v>
       </c>
@@ -3476,9 +4473,7 @@
       <c r="D40" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="E40" s="28"/>
       <c r="I40" s="3" t="s">
         <v>80</v>
       </c>
@@ -3489,10 +4484,13 @@
         <v>80</v>
       </c>
       <c r="L40" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M40" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>138</v>
       </c>
@@ -3505,14 +4503,15 @@
       <c r="D41" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H41" s="3">
+      <c r="E41" s="28"/>
+      <c r="I41" s="3">
         <v>3</v>
       </c>
-      <c r="J41" s="3">
+      <c r="K41" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>138</v>
       </c>
@@ -3525,17 +4524,17 @@
       <c r="D42" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="22"/>
+      <c r="E42" s="30"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="22"/>
+      <c r="I42" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22" t="s">
+      <c r="J42" s="22"/>
+      <c r="K42" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K42" s="22"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -3558,8 +4557,9 @@
       <c r="AE42" s="22"/>
       <c r="AF42" s="22"/>
       <c r="AG42" s="22"/>
-    </row>
-    <row r="43" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH42" s="22"/>
+    </row>
+    <row r="43" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>138</v>
       </c>
@@ -3572,27 +4572,27 @@
       <c r="D43" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="25">
-        <v>1</v>
-      </c>
+      <c r="E43" s="28"/>
       <c r="F43" s="25">
         <v>1</v>
       </c>
       <c r="G43" s="25">
         <v>1</v>
       </c>
-      <c r="H43" s="25"/>
+      <c r="H43" s="25">
+        <v>1</v>
+      </c>
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
       <c r="L43" s="25"/>
-      <c r="M43" s="25">
-        <v>1</v>
-      </c>
+      <c r="M43" s="25"/>
       <c r="N43" s="25">
         <v>1</v>
       </c>
-      <c r="O43" s="25"/>
+      <c r="O43" s="25">
+        <v>1</v>
+      </c>
       <c r="P43" s="25"/>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
@@ -3611,8 +4611,9 @@
       <c r="AE43" s="25"/>
       <c r="AF43" s="25"/>
       <c r="AG43" s="25"/>
-    </row>
-    <row r="44" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH43" s="25"/>
+    </row>
+    <row r="44" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>138</v>
       </c>
@@ -3625,27 +4626,27 @@
       <c r="D44" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="E44" s="28"/>
       <c r="F44" s="3" t="s">
         <v>77</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H44" s="25"/>
+      <c r="H44" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="I44" s="25"/>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
-      <c r="M44" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="M44" s="25"/>
       <c r="N44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O44" s="25"/>
+      <c r="O44" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="P44" s="25"/>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
@@ -3664,8 +4665,9 @@
       <c r="AE44" s="25"/>
       <c r="AF44" s="25"/>
       <c r="AG44" s="25"/>
-    </row>
-    <row r="45" spans="1:33" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH44" s="25"/>
+    </row>
+    <row r="45" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>138</v>
       </c>
@@ -3678,16 +4680,16 @@
       <c r="D45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="28"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="3"/>
       <c r="I45" s="25"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="3"/>
       <c r="O45" s="25"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
@@ -3707,8 +4709,9 @@
       <c r="AE45" s="25"/>
       <c r="AF45" s="25"/>
       <c r="AG45" s="25"/>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH45" s="25"/>
+    </row>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>138</v>
       </c>
@@ -3721,8 +4724,9 @@
       <c r="D46" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E46" s="28"/>
+    </row>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>138</v>
       </c>
@@ -3735,8 +4739,11 @@
       <c r="D47" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E47" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>138</v>
       </c>
@@ -3749,23 +4756,24 @@
       <c r="D48" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="O48" s="3">
+      <c r="E48" s="28"/>
+      <c r="P48" s="3">
         <v>0.98</v>
       </c>
-      <c r="Q48" s="3">
+      <c r="R48" s="3">
         <v>0.98229999999999995</v>
       </c>
-      <c r="R48" s="3">
+      <c r="S48" s="3">
         <v>0.98</v>
       </c>
-      <c r="X48" s="3">
+      <c r="Y48" s="3">
         <v>0.97499999999999998</v>
       </c>
-      <c r="Z48" s="3">
+      <c r="AA48" s="3">
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>138</v>
       </c>
@@ -3778,8 +4786,11 @@
       <c r="D49" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="E49" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>138</v>
       </c>
@@ -3792,23 +4803,24 @@
       <c r="D50" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="3">
-        <v>2</v>
-      </c>
+      <c r="E50" s="28"/>
       <c r="F50" s="3">
         <v>2</v>
       </c>
       <c r="G50" s="3">
         <v>2</v>
       </c>
-      <c r="M50" s="3">
+      <c r="H50" s="3">
         <v>2</v>
       </c>
       <c r="N50" s="3">
+        <v>2</v>
+      </c>
+      <c r="O50" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>138</v>
       </c>
@@ -3821,23 +4833,24 @@
       <c r="D51" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="E51" s="28"/>
       <c r="F51" s="3" t="s">
         <v>80</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M51" s="3" t="s">
+      <c r="H51" s="3" t="s">
         <v>80</v>
       </c>
       <c r="N51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O51" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>138</v>
       </c>
@@ -3850,14 +4863,15 @@
       <c r="D52" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="28"/>
+      <c r="F52" s="3">
         <v>3</v>
       </c>
-      <c r="G52" s="3">
+      <c r="H52" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:33" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>138</v>
       </c>
@@ -3870,14 +4884,14 @@
       <c r="D53" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E53" s="22" t="s">
+      <c r="E53" s="30"/>
+      <c r="F53" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22" t="s">
+      <c r="G53" s="22"/>
+      <c r="H53" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H53" s="22"/>
       <c r="I53" s="22"/>
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
@@ -3903,355 +4917,446 @@
       <c r="AE53" s="22"/>
       <c r="AF53" s="22"/>
       <c r="AG53" s="22"/>
+      <c r="AH53" s="22"/>
+    </row>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E55" s="16"/>
+    </row>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E57" s="16"/>
+    </row>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E58" s="16"/>
+    </row>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E59" s="16"/>
+    </row>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E60" s="16"/>
+    </row>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E61" s="16"/>
+    </row>
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E63" s="16"/>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="E64" s="16"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="16"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="16"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="16"/>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="16"/>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="16"/>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="16"/>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="16"/>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="16"/>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="16"/>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="16"/>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="16"/>
+    </row>
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E77" s="16"/>
+    </row>
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E78" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:D6 C7:D9 A14:D15 A13:C13 A18:D18 A11:D11 D10">
-    <cfRule type="expression" dxfId="68" priority="139">
+    <cfRule type="expression" dxfId="189" priority="177">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="67" priority="132">
+    <cfRule type="expression" dxfId="188" priority="170">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16">
-    <cfRule type="expression" dxfId="66" priority="115">
+    <cfRule type="expression" dxfId="187" priority="153">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14">
-    <cfRule type="expression" dxfId="65" priority="127">
+    <cfRule type="expression" dxfId="186" priority="165">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="64" priority="113">
+    <cfRule type="expression" dxfId="185" priority="151">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="63" priority="100">
+    <cfRule type="expression" dxfId="184" priority="138">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="62" priority="117">
+    <cfRule type="expression" dxfId="183" priority="155">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="61" priority="114">
+    <cfRule type="expression" dxfId="182" priority="152">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B20">
-    <cfRule type="expression" dxfId="60" priority="118">
+    <cfRule type="expression" dxfId="181" priority="156">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="59" priority="116">
+    <cfRule type="expression" dxfId="180" priority="154">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="58" priority="102">
+    <cfRule type="expression" dxfId="179" priority="140">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="57" priority="101">
+    <cfRule type="expression" dxfId="178" priority="139">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:C10">
-    <cfRule type="expression" dxfId="56" priority="69">
+    <cfRule type="expression" dxfId="177" priority="107">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:D17">
-    <cfRule type="expression" dxfId="55" priority="68">
+    <cfRule type="expression" dxfId="176" priority="106">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:D19">
-    <cfRule type="expression" dxfId="54" priority="64">
+    <cfRule type="expression" dxfId="175" priority="102">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D26 C24 C29:D29 C22:D22 D21">
-    <cfRule type="expression" dxfId="53" priority="63">
+    <cfRule type="expression" dxfId="174" priority="101">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25">
-    <cfRule type="expression" dxfId="52" priority="62">
+    <cfRule type="expression" dxfId="173" priority="100">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="51" priority="56">
+    <cfRule type="expression" dxfId="172" priority="94">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="50" priority="53">
+    <cfRule type="expression" dxfId="171" priority="91">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="49" priority="60">
+    <cfRule type="expression" dxfId="170" priority="98">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="48" priority="57">
+    <cfRule type="expression" dxfId="169" priority="95">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="47" priority="59">
+    <cfRule type="expression" dxfId="168" priority="97">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="46" priority="54">
+    <cfRule type="expression" dxfId="167" priority="92">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="45" priority="52">
+    <cfRule type="expression" dxfId="166" priority="90">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D28">
-    <cfRule type="expression" dxfId="44" priority="51">
+    <cfRule type="expression" dxfId="165" priority="89">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:D30">
-    <cfRule type="expression" dxfId="43" priority="50">
+    <cfRule type="expression" dxfId="164" priority="88">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:D37 C35 C40:D40 C33:D33 D32">
-    <cfRule type="expression" dxfId="42" priority="49">
+    <cfRule type="expression" dxfId="163" priority="87">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="expression" dxfId="41" priority="48">
+    <cfRule type="expression" dxfId="162" priority="86">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="40" priority="42">
+    <cfRule type="expression" dxfId="161" priority="80">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="39" priority="39">
+    <cfRule type="expression" dxfId="160" priority="77">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="38" priority="46">
+    <cfRule type="expression" dxfId="159" priority="84">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="158" priority="81">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="36" priority="45">
+    <cfRule type="expression" dxfId="157" priority="83">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="35" priority="40">
+    <cfRule type="expression" dxfId="156" priority="78">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="34" priority="38">
+    <cfRule type="expression" dxfId="155" priority="76">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:D39">
-    <cfRule type="expression" dxfId="33" priority="37">
+    <cfRule type="expression" dxfId="154" priority="75">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:D41">
-    <cfRule type="expression" dxfId="32" priority="36">
+    <cfRule type="expression" dxfId="153" priority="74">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:D48 C46 C51:D51 C44:D44 D43">
-    <cfRule type="expression" dxfId="31" priority="35">
+    <cfRule type="expression" dxfId="152" priority="73">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
-    <cfRule type="expression" dxfId="30" priority="34">
+    <cfRule type="expression" dxfId="151" priority="72">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="150" priority="66">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="28" priority="25">
+    <cfRule type="expression" dxfId="149" priority="63">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="148" priority="70">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="26" priority="29">
+    <cfRule type="expression" dxfId="147" priority="67">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="25" priority="31">
+    <cfRule type="expression" dxfId="146" priority="69">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="24" priority="26">
+    <cfRule type="expression" dxfId="145" priority="64">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="144" priority="62">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:D50">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="143" priority="61">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:D52">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="142" priority="60">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:B26 A29:B29 A22:B22">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="141" priority="59">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="19" priority="19">
+    <cfRule type="expression" dxfId="140" priority="57">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31">
-    <cfRule type="expression" dxfId="18" priority="20">
+    <cfRule type="expression" dxfId="139" priority="58">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:B23">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="138" priority="56">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="137" priority="55">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="136" priority="54">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B37 A40:B40 A33:B33">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="135" priority="53">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B38">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="134" priority="51">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="133" priority="52">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B34">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="132" priority="50">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="131" priority="49">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="130" priority="48">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:B41">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="129" priority="47">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:B48 A51:B51 A44:B44">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="128" priority="46">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="127" priority="44">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:B53">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="126" priority="45">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:B45">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="125" priority="43">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B43">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="124" priority="42">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="123" priority="41">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:B52">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="122" priority="40">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:B21">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="121" priority="39">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="expression" dxfId="120" priority="37">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:E9">
+    <cfRule type="expression" dxfId="119" priority="36">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E53">
+    <cfRule type="expression" dxfId="107" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:N6" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:O6" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
       <formula1>TEST_OUTCOME_TYPES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated code to track unit types for both the RMR and TCD descriptions. A new json called "unit_conventions.json" will track the display names for various unit types.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/transformer_tests_draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94AAC10-D135-4B5F-8982-45E6264A9828}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68381806-16AB-48C1-AE64-DC80BCEF5AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="145">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -466,7 +466,16 @@
     <t>W</t>
   </si>
   <si>
-    <t>V*A</t>
+    <t>unit_type</t>
+  </si>
+  <si>
+    <t>V-A</t>
+  </si>
+  <si>
+    <t>transformer_capacity</t>
+  </si>
+  <si>
+    <t>electric_power</t>
   </si>
 </sst>
 </file>
@@ -748,49 +757,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="190">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="75">
     <dxf>
       <fill>
         <patternFill>
@@ -815,770 +782,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2389,13 +1593,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
-  <dimension ref="A1:AJ78"/>
+  <dimension ref="A1:AK78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH7" sqref="AH7"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,18 +1608,19 @@
     <col min="2" max="2" width="17.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="52.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="34" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="52.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="53.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="51.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="35" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
@@ -2429,100 +1634,103 @@
         <v>64</v>
       </c>
       <c r="E1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="5" t="str">
-        <f>"rule-"&amp;F2&amp;"-"&amp;F3&amp;F4</f>
+      <c r="G1" s="5" t="str">
+        <f>"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
         <v>rule-15-1a</v>
       </c>
-      <c r="G1" s="5" t="str">
-        <f t="shared" ref="G1:H1" si="0">"rule-"&amp;G2&amp;"-"&amp;G3&amp;G4</f>
+      <c r="H1" s="5" t="str">
+        <f t="shared" ref="H1:I1" si="0">"rule-"&amp;H2&amp;"-"&amp;H3&amp;H4</f>
         <v>rule-15-1b</v>
       </c>
-      <c r="H1" s="5" t="str">
+      <c r="I1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-15-1c</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>69</v>
       </c>
@@ -2530,9 +1738,7 @@
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="27"/>
-      <c r="F2" s="3">
-        <v>15</v>
-      </c>
+      <c r="F2" s="27"/>
       <c r="G2" s="3">
         <v>15</v>
       </c>
@@ -2617,10 +1823,13 @@
       <c r="AH2" s="3">
         <v>15</v>
       </c>
-      <c r="AI2" s="3"/>
+      <c r="AI2" s="3">
+        <v>15</v>
+      </c>
       <c r="AJ2" s="3"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK2" s="3"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
@@ -2628,9 +1837,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="27"/>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
+      <c r="F3" s="27"/>
       <c r="G3" s="3">
         <v>1</v>
       </c>
@@ -2638,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="3">
         <v>2</v>
@@ -2647,19 +1854,19 @@
         <v>2</v>
       </c>
       <c r="L3" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M3" s="3">
         <v>3</v>
       </c>
       <c r="N3" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O3" s="3">
         <v>4</v>
       </c>
       <c r="P3" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q3" s="3">
         <v>5</v>
@@ -2671,7 +1878,7 @@
         <v>5</v>
       </c>
       <c r="T3" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U3" s="3">
         <v>6</v>
@@ -2683,7 +1890,7 @@
         <v>6</v>
       </c>
       <c r="X3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y3" s="3">
         <v>7</v>
@@ -2695,7 +1902,7 @@
         <v>7</v>
       </c>
       <c r="AB3" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC3" s="3">
         <v>8</v>
@@ -2715,10 +1922,13 @@
       <c r="AH3" s="3">
         <v>8</v>
       </c>
-      <c r="AI3" s="3"/>
+      <c r="AI3" s="3">
+        <v>8</v>
+      </c>
       <c r="AJ3" s="3"/>
-    </row>
-    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK3" s="3"/>
+    </row>
+    <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>55</v>
       </c>
@@ -2726,97 +1936,98 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="27"/>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
-    </row>
-    <row r="5" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+      <c r="AK4" s="3"/>
+    </row>
+    <row r="5" spans="1:37" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -2824,95 +2035,96 @@
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="28"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="T5" s="4" t="s">
+      <c r="U5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
@@ -2920,97 +2132,98 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="29"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="29"/>
+      <c r="G6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="V6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="3" t="s">
+      <c r="W6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="W6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X6" s="3" t="s">
+      <c r="Y6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Z6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Z6" s="3" t="s">
+      <c r="AA6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AH6" s="3" t="s">
+      <c r="AI6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
-    </row>
-    <row r="7" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AK6" s="3"/>
+    </row>
+    <row r="7" spans="1:37" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>68</v>
       </c>
@@ -3020,7 +2233,7 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -3030,10 +2243,7 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
-      <c r="P7" s="19" t="str">
-        <f>"true"</f>
-        <v>true</v>
-      </c>
+      <c r="P7" s="19"/>
       <c r="Q7" s="19" t="str">
         <f>"true"</f>
         <v>true</v>
@@ -3046,56 +2256,60 @@
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="T7" s="19"/>
+      <c r="T7" s="19" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
       <c r="W7" s="19"/>
-      <c r="X7" s="19" t="str">
-        <f>"true"</f>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19" t="str">
+        <f t="shared" ref="Y7:AI7" si="1">"true"</f>
         <v>true</v>
       </c>
-      <c r="Y7" s="19" t="str">
-        <f>"true"</f>
+      <c r="Z7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="Z7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AA7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AA7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AB7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AB7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AC7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AC7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AD7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AD7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AE7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AE7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AF7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AF7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AG7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AG7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AH7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
-      <c r="AH7" s="19" t="str">
-        <f>"true"</f>
+      <c r="AI7" s="19" t="str">
+        <f t="shared" si="1"/>
         <v>true</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
@@ -3105,7 +2319,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="28"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -3127,36 +2341,37 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
-      <c r="AB8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4" t="str">
+        <f t="shared" ref="AC8:AI8" si="2">"true"</f>
         <v>true</v>
       </c>
-      <c r="AC8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AD8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="AD8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AE8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="AE8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AF8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="AF8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AG8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="AG8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AH8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
-      <c r="AH8" s="4" t="str">
-        <f>"true"</f>
+      <c r="AI8" s="4" t="str">
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
     </row>
-    <row r="9" spans="1:36" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>68</v>
       </c>
@@ -3166,20 +2381,17 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="29"/>
-      <c r="F9" s="22"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
-      <c r="N9" s="22"/>
+      <c r="N9" s="23"/>
       <c r="O9" s="22"/>
-      <c r="P9" s="22" t="str">
-        <f>"true"</f>
-        <v>true</v>
-      </c>
+      <c r="P9" s="22"/>
       <c r="Q9" s="22" t="str">
         <f>"true"</f>
         <v>true</v>
@@ -3192,14 +2404,14 @@
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="T9" s="22"/>
+      <c r="T9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="U9" s="22"/>
       <c r="V9" s="22"/>
       <c r="W9" s="22"/>
-      <c r="X9" s="22" t="str">
-        <f>"true"</f>
-        <v>true</v>
-      </c>
+      <c r="X9" s="22"/>
       <c r="Y9" s="22" t="str">
         <f>"true"</f>
         <v>true</v>
@@ -3212,15 +2424,19 @@
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="AB9" s="22"/>
+      <c r="AB9" s="22" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
       <c r="AC9" s="22"/>
       <c r="AD9" s="22"/>
       <c r="AE9" s="22"/>
       <c r="AF9" s="22"/>
       <c r="AG9" s="22"/>
       <c r="AH9" s="22"/>
-    </row>
-    <row r="10" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI9" s="22"/>
+    </row>
+    <row r="10" spans="1:37" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>68</v>
       </c>
@@ -3234,20 +2450,17 @@
         <v>137</v>
       </c>
       <c r="E10" s="28"/>
-      <c r="F10" s="25"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="25"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="25"/>
+      <c r="N10" s="4"/>
       <c r="O10" s="25"/>
-      <c r="P10" s="25" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
+      <c r="P10" s="25"/>
       <c r="Q10" s="25" t="str">
         <f>"1"</f>
         <v>1</v>
@@ -3260,56 +2473,60 @@
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="T10" s="25"/>
+      <c r="T10" s="25" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
       <c r="W10" s="25"/>
-      <c r="X10" s="25" t="str">
-        <f t="shared" ref="X10:AH10" si="1">"1"</f>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25" t="str">
+        <f t="shared" ref="Y10:AI10" si="3">"1"</f>
         <v>1</v>
       </c>
-      <c r="Y10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="Z10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="Z10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AA10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AA10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AB10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AB10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AC10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AD10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AD10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AE10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AE10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AF10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AF10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AG10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AG10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AH10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AH10" s="25" t="str">
-        <f t="shared" si="1"/>
+      <c r="AI10" s="25" t="str">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>68</v>
       </c>
@@ -3323,9 +2540,7 @@
         <v>72</v>
       </c>
       <c r="E11" s="28"/>
-      <c r="P11" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F11" s="28"/>
       <c r="Q11" s="3" t="s">
         <v>77</v>
       </c>
@@ -3335,7 +2550,7 @@
       <c r="S11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="X11" s="3" t="s">
+      <c r="T11" s="3" t="s">
         <v>77</v>
       </c>
       <c r="Y11" s="3" t="s">
@@ -3368,8 +2583,11 @@
       <c r="AH11" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AI11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
@@ -3383,9 +2601,7 @@
         <v>87</v>
       </c>
       <c r="E12" s="28"/>
-      <c r="P12" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="F12" s="28"/>
       <c r="Q12" s="3" t="s">
         <v>88</v>
       </c>
@@ -3395,26 +2611,26 @@
       <c r="S12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="X12" s="3" t="s">
-        <v>95</v>
+      <c r="T12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="Y12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>88</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="AC12" s="3" t="s">
         <v>95</v>
       </c>
       <c r="AD12" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>88</v>
@@ -3428,8 +2644,11 @@
       <c r="AH12" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AI12" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>68</v>
       </c>
@@ -3443,41 +2662,39 @@
         <v>73</v>
       </c>
       <c r="E13" s="28"/>
-      <c r="P13" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="F13" s="28"/>
       <c r="Q13" s="3" t="s">
         <v>89</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="X13" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="Y13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>89</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC13" s="3" t="s">
         <v>90</v>
       </c>
       <c r="AD13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE13" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="AE13" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="AF13" s="3" t="s">
         <v>90</v>
@@ -3485,8 +2702,11 @@
       <c r="AG13" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AH13" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
@@ -3500,40 +2720,40 @@
         <v>75</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="P14" s="3">
-        <v>25000</v>
+        <v>143</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>142</v>
       </c>
       <c r="Q14" s="3">
         <v>25000</v>
       </c>
       <c r="R14" s="3">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="S14" s="3">
         <v>30000</v>
       </c>
-      <c r="X14" s="3">
+      <c r="T14" s="3">
         <v>30000</v>
       </c>
       <c r="Y14" s="3">
         <v>30000</v>
       </c>
       <c r="Z14" s="3">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="AA14" s="3">
         <v>25000</v>
       </c>
       <c r="AB14" s="3">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="AC14" s="3">
         <v>30000</v>
       </c>
       <c r="AD14" s="3">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="AE14" s="3">
         <v>25000</v>
@@ -3547,8 +2767,11 @@
       <c r="AH14" s="3">
         <v>25000</v>
       </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AI14" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>68</v>
       </c>
@@ -3562,29 +2785,30 @@
         <v>74</v>
       </c>
       <c r="E15" s="28"/>
-      <c r="Q15" s="3">
+      <c r="F15" s="28"/>
+      <c r="R15" s="3">
         <v>0.99</v>
       </c>
-      <c r="X15" s="3">
+      <c r="Y15" s="3">
         <v>0.98</v>
       </c>
-      <c r="Z15" s="3">
+      <c r="AA15" s="3">
         <v>0.98</v>
       </c>
-      <c r="AB15" s="3">
+      <c r="AC15" s="3">
         <v>0.98</v>
       </c>
-      <c r="AD15" s="3">
+      <c r="AE15" s="3">
         <v>0.99</v>
       </c>
-      <c r="AF15" s="3">
+      <c r="AG15" s="3">
         <v>0.99</v>
       </c>
-      <c r="AH15" s="3">
+      <c r="AI15" s="3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>68</v>
       </c>
@@ -3598,10 +2822,13 @@
         <v>76</v>
       </c>
       <c r="E16" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>68</v>
       </c>
@@ -3615,8 +2842,9 @@
         <v>137</v>
       </c>
       <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>68</v>
       </c>
@@ -3630,8 +2858,9 @@
         <v>72</v>
       </c>
       <c r="E18" s="28"/>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>68</v>
       </c>
@@ -3645,8 +2874,9 @@
         <v>137</v>
       </c>
       <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>68</v>
       </c>
@@ -3660,7 +2890,7 @@
         <v>72</v>
       </c>
       <c r="E20" s="30"/>
-      <c r="F20" s="22"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
@@ -3689,8 +2919,9 @@
       <c r="AF20" s="22"/>
       <c r="AG20" s="22"/>
       <c r="AH20" s="22"/>
-    </row>
-    <row r="21" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI20" s="22"/>
+    </row>
+    <row r="21" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>138</v>
       </c>
@@ -3704,54 +2935,51 @@
         <v>137</v>
       </c>
       <c r="E21" s="28"/>
-      <c r="F21" s="25" t="str">
-        <f t="shared" ref="F21:O21" si="2">"1"</f>
+      <c r="F21" s="28"/>
+      <c r="G21" s="25" t="str">
+        <f t="shared" ref="G21:P21" si="4">"1"</f>
         <v>1</v>
       </c>
-      <c r="G21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="H21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="I21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="J21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="K21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="L21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="M21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="N21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="O21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O21" s="25" t="str">
-        <f t="shared" si="2"/>
+      <c r="P21" s="25" t="str">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P21" s="25"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
-      <c r="T21" s="25" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
+      <c r="T21" s="25"/>
       <c r="U21" s="25" t="str">
         <f>"1"</f>
         <v>1</v>
@@ -3764,7 +2992,10 @@
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="X21" s="25"/>
+      <c r="X21" s="25" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="Y21" s="25"/>
       <c r="Z21" s="25"/>
       <c r="AA21" s="25"/>
@@ -3775,8 +3006,9 @@
       <c r="AF21" s="25"/>
       <c r="AG21" s="25"/>
       <c r="AH21" s="25"/>
-    </row>
-    <row r="22" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI21" s="25"/>
+    </row>
+    <row r="22" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>138</v>
       </c>
@@ -3790,9 +3022,7 @@
         <v>72</v>
       </c>
       <c r="E22" s="28"/>
-      <c r="F22" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F22" s="28"/>
       <c r="G22" s="3" t="s">
         <v>77</v>
       </c>
@@ -3820,13 +3050,13 @@
       <c r="O22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P22" s="25"/>
+      <c r="P22" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
-      <c r="T22" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="T22" s="25"/>
       <c r="U22" s="3" t="s">
         <v>77</v>
       </c>
@@ -3836,7 +3066,9 @@
       <c r="W22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="X22" s="3"/>
+      <c r="X22" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
@@ -3847,8 +3079,9 @@
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
-    </row>
-    <row r="23" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI22" s="3"/>
+    </row>
+    <row r="23" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>138</v>
       </c>
@@ -3862,23 +3095,21 @@
         <v>87</v>
       </c>
       <c r="E23" s="28"/>
-      <c r="F23" s="3"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="25"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="3"/>
       <c r="P23" s="25"/>
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
-      <c r="T23" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="T23" s="25"/>
       <c r="U23" s="3" t="s">
         <v>88</v>
       </c>
@@ -3888,7 +3119,9 @@
       <c r="W23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="X23" s="3"/>
+      <c r="X23" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
@@ -3899,8 +3132,9 @@
       <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI23" s="3"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>138</v>
       </c>
@@ -3914,29 +3148,30 @@
         <v>73</v>
       </c>
       <c r="E24" s="28"/>
-      <c r="M24" s="6"/>
-      <c r="O24" s="6"/>
+      <c r="F24" s="28"/>
+      <c r="N24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="T24" s="6"/>
       <c r="U24" s="3" t="s">
         <v>89</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AH24" s="3" t="s">
+      <c r="X24" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI24" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>138</v>
       </c>
@@ -3950,10 +3185,10 @@
         <v>75</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="T25" s="3">
-        <v>25000</v>
+        <v>143</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>142</v>
       </c>
       <c r="U25" s="3">
         <v>25000</v>
@@ -3964,8 +3199,11 @@
       <c r="W25" s="3">
         <v>25000</v>
       </c>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="X25" s="3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>138</v>
       </c>
@@ -3979,44 +3217,45 @@
         <v>74</v>
       </c>
       <c r="E26" s="28"/>
-      <c r="P26" s="3">
-        <v>0.99</v>
-      </c>
-      <c r="R26" s="3">
+      <c r="F26" s="28"/>
+      <c r="Q26" s="3">
         <v>0.99</v>
       </c>
       <c r="S26" s="3">
         <v>0.99</v>
       </c>
       <c r="T26" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="U26" s="3">
         <v>0.98</v>
       </c>
-      <c r="U26" s="3">
+      <c r="V26" s="3">
         <v>0.97</v>
       </c>
-      <c r="V26" s="3">
+      <c r="W26" s="3">
         <v>0.98299999999999998</v>
       </c>
-      <c r="W26" s="3">
+      <c r="X26" s="3">
         <v>0.98</v>
       </c>
-      <c r="Y26" s="3">
+      <c r="Z26" s="3">
         <v>0.98</v>
       </c>
-      <c r="AA26" s="3">
+      <c r="AB26" s="3">
         <v>0.98</v>
       </c>
-      <c r="AC26" s="3">
+      <c r="AD26" s="3">
         <v>0.98</v>
       </c>
-      <c r="AE26" s="3">
+      <c r="AF26" s="3">
         <v>0.99</v>
       </c>
-      <c r="AG26" s="3">
+      <c r="AH26" s="3">
         <v>0.99</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>138</v>
       </c>
@@ -4030,10 +3269,13 @@
         <v>76</v>
       </c>
       <c r="E27" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>138</v>
       </c>
@@ -4047,9 +3289,7 @@
         <v>137</v>
       </c>
       <c r="E28" s="28"/>
-      <c r="F28" s="3">
-        <v>2</v>
-      </c>
+      <c r="F28" s="28"/>
       <c r="G28" s="3">
         <v>2</v>
       </c>
@@ -4077,8 +3317,11 @@
       <c r="O28" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="P28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>138</v>
       </c>
@@ -4092,9 +3335,7 @@
         <v>72</v>
       </c>
       <c r="E29" s="28"/>
-      <c r="F29" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F29" s="28"/>
       <c r="G29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4122,8 +3363,11 @@
       <c r="O29" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="P29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>138</v>
       </c>
@@ -4137,20 +3381,21 @@
         <v>137</v>
       </c>
       <c r="E30" s="28"/>
-      <c r="F30" s="3">
-        <v>3</v>
-      </c>
+      <c r="F30" s="28"/>
       <c r="G30" s="3">
         <v>3</v>
       </c>
-      <c r="I30" s="3">
+      <c r="H30" s="3">
         <v>3</v>
       </c>
       <c r="J30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>138</v>
       </c>
@@ -4164,20 +3409,20 @@
         <v>72</v>
       </c>
       <c r="E31" s="30"/>
-      <c r="F31" s="22" t="s">
-        <v>81</v>
-      </c>
+      <c r="F31" s="30"/>
       <c r="G31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22" t="s">
+      <c r="H31" s="22" t="s">
         <v>81</v>
       </c>
+      <c r="I31" s="22"/>
       <c r="J31" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="K31" s="22"/>
+      <c r="K31" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
@@ -4201,8 +3446,9 @@
       <c r="AF31" s="22"/>
       <c r="AG31" s="22"/>
       <c r="AH31" s="22"/>
-    </row>
-    <row r="32" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI31" s="22"/>
+    </row>
+    <row r="32" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>138</v>
       </c>
@@ -4216,12 +3462,10 @@
         <v>137</v>
       </c>
       <c r="E32" s="28"/>
-      <c r="F32" s="25"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
-      <c r="I32" s="25">
-        <v>1</v>
-      </c>
+      <c r="I32" s="25"/>
       <c r="J32" s="25">
         <v>1</v>
       </c>
@@ -4234,7 +3478,9 @@
       <c r="M32" s="25">
         <v>1</v>
       </c>
-      <c r="N32" s="25"/>
+      <c r="N32" s="25">
+        <v>1</v>
+      </c>
       <c r="O32" s="25"/>
       <c r="P32" s="25"/>
       <c r="Q32" s="25"/>
@@ -4255,8 +3501,9 @@
       <c r="AF32" s="25"/>
       <c r="AG32" s="25"/>
       <c r="AH32" s="25"/>
-    </row>
-    <row r="33" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI32" s="25"/>
+    </row>
+    <row r="33" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>138</v>
       </c>
@@ -4270,12 +3517,10 @@
         <v>72</v>
       </c>
       <c r="E33" s="28"/>
-      <c r="F33" s="25"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
-      <c r="I33" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="I33" s="25"/>
       <c r="J33" s="3" t="s">
         <v>77</v>
       </c>
@@ -4288,7 +3533,9 @@
       <c r="M33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="N33" s="25"/>
+      <c r="N33" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="O33" s="25"/>
       <c r="P33" s="25"/>
       <c r="Q33" s="25"/>
@@ -4309,8 +3556,9 @@
       <c r="AF33" s="25"/>
       <c r="AG33" s="25"/>
       <c r="AH33" s="25"/>
-    </row>
-    <row r="34" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI33" s="25"/>
+    </row>
+    <row r="34" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>138</v>
       </c>
@@ -4324,14 +3572,14 @@
         <v>87</v>
       </c>
       <c r="E34" s="28"/>
-      <c r="F34" s="25"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="25"/>
+      <c r="M34" s="3"/>
       <c r="N34" s="25"/>
       <c r="O34" s="25"/>
       <c r="P34" s="25"/>
@@ -4353,8 +3601,9 @@
       <c r="AF34" s="25"/>
       <c r="AG34" s="25"/>
       <c r="AH34" s="25"/>
-    </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI34" s="25"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>138</v>
       </c>
@@ -4368,11 +3617,12 @@
         <v>73</v>
       </c>
       <c r="E35" s="28"/>
-      <c r="AH35" s="3" t="s">
+      <c r="F35" s="28"/>
+      <c r="AI35" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>138</v>
       </c>
@@ -4386,10 +3636,13 @@
         <v>75</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>138</v>
       </c>
@@ -4403,17 +3656,18 @@
         <v>74</v>
       </c>
       <c r="E37" s="28"/>
-      <c r="AC37" s="3">
+      <c r="F37" s="28"/>
+      <c r="AD37" s="3">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AE37" s="3">
+      <c r="AF37" s="3">
         <v>0.98</v>
       </c>
-      <c r="AG37" s="3">
+      <c r="AH37" s="3">
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>138</v>
       </c>
@@ -4427,10 +3681,13 @@
         <v>76</v>
       </c>
       <c r="E38" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>138</v>
       </c>
@@ -4444,9 +3701,7 @@
         <v>137</v>
       </c>
       <c r="E39" s="28"/>
-      <c r="I39" s="3">
-        <v>2</v>
-      </c>
+      <c r="F39" s="28"/>
       <c r="J39" s="3">
         <v>2</v>
       </c>
@@ -4457,10 +3712,13 @@
         <v>2</v>
       </c>
       <c r="M39" s="3">
+        <v>2</v>
+      </c>
+      <c r="N39" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>138</v>
       </c>
@@ -4474,9 +3732,7 @@
         <v>72</v>
       </c>
       <c r="E40" s="28"/>
-      <c r="I40" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F40" s="28"/>
       <c r="J40" s="3" t="s">
         <v>80</v>
       </c>
@@ -4487,10 +3743,13 @@
         <v>80</v>
       </c>
       <c r="M40" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N40" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>138</v>
       </c>
@@ -4504,14 +3763,15 @@
         <v>137</v>
       </c>
       <c r="E41" s="28"/>
-      <c r="I41" s="3">
+      <c r="F41" s="28"/>
+      <c r="J41" s="3">
         <v>3</v>
       </c>
-      <c r="K41" s="3">
+      <c r="L41" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>138</v>
       </c>
@@ -4525,17 +3785,17 @@
         <v>72</v>
       </c>
       <c r="E42" s="30"/>
-      <c r="F42" s="22"/>
+      <c r="F42" s="30"/>
       <c r="G42" s="22"/>
       <c r="H42" s="22"/>
-      <c r="I42" s="22" t="s">
+      <c r="I42" s="22"/>
+      <c r="J42" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22" t="s">
+      <c r="K42" s="22"/>
+      <c r="L42" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -4558,8 +3818,9 @@
       <c r="AF42" s="22"/>
       <c r="AG42" s="22"/>
       <c r="AH42" s="22"/>
-    </row>
-    <row r="43" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI42" s="22"/>
+    </row>
+    <row r="43" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>138</v>
       </c>
@@ -4573,27 +3834,27 @@
         <v>137</v>
       </c>
       <c r="E43" s="28"/>
-      <c r="F43" s="25">
-        <v>1</v>
-      </c>
+      <c r="F43" s="28"/>
       <c r="G43" s="25">
         <v>1</v>
       </c>
       <c r="H43" s="25">
         <v>1</v>
       </c>
-      <c r="I43" s="25"/>
+      <c r="I43" s="25">
+        <v>1</v>
+      </c>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
-      <c r="N43" s="25">
-        <v>1</v>
-      </c>
+      <c r="N43" s="25"/>
       <c r="O43" s="25">
         <v>1</v>
       </c>
-      <c r="P43" s="25"/>
+      <c r="P43" s="25">
+        <v>1</v>
+      </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
@@ -4612,8 +3873,9 @@
       <c r="AF43" s="25"/>
       <c r="AG43" s="25"/>
       <c r="AH43" s="25"/>
-    </row>
-    <row r="44" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI43" s="25"/>
+    </row>
+    <row r="44" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>138</v>
       </c>
@@ -4627,27 +3889,27 @@
         <v>72</v>
       </c>
       <c r="E44" s="28"/>
-      <c r="F44" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="F44" s="28"/>
       <c r="G44" s="3" t="s">
         <v>77</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I44" s="25"/>
+      <c r="I44" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
-      <c r="N44" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="N44" s="25"/>
       <c r="O44" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P44" s="25"/>
+      <c r="P44" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
@@ -4666,8 +3928,9 @@
       <c r="AF44" s="25"/>
       <c r="AG44" s="25"/>
       <c r="AH44" s="25"/>
-    </row>
-    <row r="45" spans="1:34" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AI44" s="25"/>
+    </row>
+    <row r="45" spans="1:35" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>138</v>
       </c>
@@ -4681,16 +3944,16 @@
         <v>87</v>
       </c>
       <c r="E45" s="28"/>
-      <c r="F45" s="3"/>
+      <c r="F45" s="28"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="25"/>
+      <c r="I45" s="3"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="3"/>
       <c r="P45" s="25"/>
       <c r="Q45" s="25"/>
       <c r="R45" s="25"/>
@@ -4710,8 +3973,9 @@
       <c r="AF45" s="25"/>
       <c r="AG45" s="25"/>
       <c r="AH45" s="25"/>
-    </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI45" s="25"/>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>138</v>
       </c>
@@ -4725,8 +3989,9 @@
         <v>73</v>
       </c>
       <c r="E46" s="28"/>
-    </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>138</v>
       </c>
@@ -4740,10 +4005,13 @@
         <v>75</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>138</v>
       </c>
@@ -4757,23 +4025,24 @@
         <v>74</v>
       </c>
       <c r="E48" s="28"/>
-      <c r="P48" s="3">
+      <c r="F48" s="28"/>
+      <c r="Q48" s="3">
         <v>0.98</v>
       </c>
-      <c r="R48" s="3">
+      <c r="S48" s="3">
         <v>0.98229999999999995</v>
       </c>
-      <c r="S48" s="3">
+      <c r="T48" s="3">
         <v>0.98</v>
       </c>
-      <c r="Y48" s="3">
+      <c r="Z48" s="3">
         <v>0.97499999999999998</v>
       </c>
-      <c r="AA48" s="3">
+      <c r="AB48" s="3">
         <v>0.98299999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>138</v>
       </c>
@@ -4787,10 +4056,13 @@
         <v>76</v>
       </c>
       <c r="E49" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>138</v>
       </c>
@@ -4804,23 +4076,24 @@
         <v>137</v>
       </c>
       <c r="E50" s="28"/>
-      <c r="F50" s="3">
-        <v>2</v>
-      </c>
+      <c r="F50" s="28"/>
       <c r="G50" s="3">
         <v>2</v>
       </c>
       <c r="H50" s="3">
         <v>2</v>
       </c>
-      <c r="N50" s="3">
+      <c r="I50" s="3">
         <v>2</v>
       </c>
       <c r="O50" s="3">
+        <v>2</v>
+      </c>
+      <c r="P50" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>138</v>
       </c>
@@ -4834,23 +4107,24 @@
         <v>72</v>
       </c>
       <c r="E51" s="28"/>
-      <c r="F51" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F51" s="28"/>
       <c r="G51" s="3" t="s">
         <v>80</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="N51" s="3" t="s">
+      <c r="I51" s="3" t="s">
         <v>80</v>
       </c>
       <c r="O51" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P51" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>138</v>
       </c>
@@ -4864,14 +4138,15 @@
         <v>137</v>
       </c>
       <c r="E52" s="28"/>
-      <c r="F52" s="3">
+      <c r="F52" s="28"/>
+      <c r="G52" s="3">
         <v>3</v>
       </c>
-      <c r="H52" s="3">
+      <c r="I52" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:34" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>138</v>
       </c>
@@ -4885,14 +4160,14 @@
         <v>72</v>
       </c>
       <c r="E53" s="30"/>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="30"/>
+      <c r="G53" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22" t="s">
+      <c r="H53" s="22"/>
+      <c r="I53" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I53" s="22"/>
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
       <c r="L53" s="22"/>
@@ -4918,445 +4193,486 @@
       <c r="AF53" s="22"/>
       <c r="AG53" s="22"/>
       <c r="AH53" s="22"/>
-    </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI53" s="22"/>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E54" s="16"/>
-    </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F54" s="16"/>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E55" s="16"/>
-    </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F55" s="16"/>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E56" s="16"/>
-    </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F56" s="16"/>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E57" s="16"/>
-    </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F57" s="16"/>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E58" s="16"/>
-    </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F58" s="16"/>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E59" s="16"/>
-    </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F59" s="16"/>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E60" s="16"/>
-    </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F60" s="16"/>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E61" s="16"/>
-    </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F61" s="16"/>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E62" s="16"/>
-    </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F62" s="16"/>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E63" s="16"/>
-    </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="F63" s="16"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E64" s="16"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="16"/>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" s="16"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E66" s="16"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E67" s="16"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68" s="16"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" s="16"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" s="16"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" s="16"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" s="16"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="16"/>
+    </row>
+    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" s="16"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="16"/>
+    </row>
+    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" s="16"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="16"/>
+    </row>
+    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E75" s="16"/>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="16"/>
+    </row>
+    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E76" s="16"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E77" s="16"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="16"/>
+    </row>
+    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:D6 C7:D9 A14:D15 A13:C13 A18:D18 A11:D11 D10">
-    <cfRule type="expression" dxfId="189" priority="177">
+    <cfRule type="expression" dxfId="74" priority="180">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="188" priority="170">
+    <cfRule type="expression" dxfId="73" priority="173">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:B16">
-    <cfRule type="expression" dxfId="187" priority="153">
+    <cfRule type="expression" dxfId="72" priority="156">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D14">
-    <cfRule type="expression" dxfId="186" priority="165">
+    <cfRule type="expression" dxfId="71" priority="168">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="185" priority="151">
+    <cfRule type="expression" dxfId="70" priority="154">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="184" priority="138">
+    <cfRule type="expression" dxfId="69" priority="141">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="183" priority="155">
+    <cfRule type="expression" dxfId="68" priority="158">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="182" priority="152">
+    <cfRule type="expression" dxfId="67" priority="155">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B20">
-    <cfRule type="expression" dxfId="181" priority="156">
+    <cfRule type="expression" dxfId="66" priority="159">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="180" priority="154">
+    <cfRule type="expression" dxfId="65" priority="157">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:B12">
-    <cfRule type="expression" dxfId="179" priority="140">
+    <cfRule type="expression" dxfId="64" priority="143">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="178" priority="139">
+    <cfRule type="expression" dxfId="63" priority="142">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:C10">
-    <cfRule type="expression" dxfId="177" priority="107">
+    <cfRule type="expression" dxfId="62" priority="110">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17:D17">
-    <cfRule type="expression" dxfId="176" priority="106">
+    <cfRule type="expression" dxfId="61" priority="109">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:D19">
-    <cfRule type="expression" dxfId="175" priority="102">
+    <cfRule type="expression" dxfId="60" priority="105">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:D26 C24 C29:D29 C22:D22 D21">
-    <cfRule type="expression" dxfId="174" priority="101">
+    <cfRule type="expression" dxfId="59" priority="104">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:D25">
-    <cfRule type="expression" dxfId="173" priority="100">
+    <cfRule type="expression" dxfId="58" priority="103">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="172" priority="94">
+    <cfRule type="expression" dxfId="57" priority="97">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="171" priority="91">
+    <cfRule type="expression" dxfId="56" priority="94">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="170" priority="98">
+    <cfRule type="expression" dxfId="55" priority="101">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="169" priority="95">
+    <cfRule type="expression" dxfId="54" priority="98">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="expression" dxfId="168" priority="97">
+    <cfRule type="expression" dxfId="53" priority="100">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="167" priority="92">
+    <cfRule type="expression" dxfId="52" priority="95">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="166" priority="90">
+    <cfRule type="expression" dxfId="51" priority="93">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D28">
-    <cfRule type="expression" dxfId="165" priority="89">
+    <cfRule type="expression" dxfId="50" priority="92">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:D30">
-    <cfRule type="expression" dxfId="164" priority="88">
+    <cfRule type="expression" dxfId="49" priority="91">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:D37 C35 C40:D40 C33:D33 D32">
-    <cfRule type="expression" dxfId="163" priority="87">
+    <cfRule type="expression" dxfId="48" priority="90">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="expression" dxfId="162" priority="86">
+    <cfRule type="expression" dxfId="47" priority="89">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="161" priority="80">
+    <cfRule type="expression" dxfId="46" priority="83">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="160" priority="77">
+    <cfRule type="expression" dxfId="45" priority="80">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="159" priority="84">
+    <cfRule type="expression" dxfId="44" priority="87">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="158" priority="81">
+    <cfRule type="expression" dxfId="43" priority="84">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42">
-    <cfRule type="expression" dxfId="157" priority="83">
+    <cfRule type="expression" dxfId="42" priority="86">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="expression" dxfId="156" priority="78">
+    <cfRule type="expression" dxfId="41" priority="81">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="expression" dxfId="155" priority="76">
+    <cfRule type="expression" dxfId="40" priority="79">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:D39">
-    <cfRule type="expression" dxfId="154" priority="75">
+    <cfRule type="expression" dxfId="39" priority="78">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:D41">
-    <cfRule type="expression" dxfId="153" priority="74">
+    <cfRule type="expression" dxfId="38" priority="77">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:D48 C46 C51:D51 C44:D44 D43">
-    <cfRule type="expression" dxfId="152" priority="73">
+    <cfRule type="expression" dxfId="37" priority="76">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:D47">
-    <cfRule type="expression" dxfId="151" priority="72">
+    <cfRule type="expression" dxfId="36" priority="75">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49">
-    <cfRule type="expression" dxfId="150" priority="66">
+    <cfRule type="expression" dxfId="35" priority="69">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="149" priority="63">
+    <cfRule type="expression" dxfId="34" priority="66">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" dxfId="148" priority="70">
+    <cfRule type="expression" dxfId="33" priority="73">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="147" priority="67">
+    <cfRule type="expression" dxfId="32" priority="70">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="146" priority="69">
+    <cfRule type="expression" dxfId="31" priority="72">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" dxfId="145" priority="64">
+    <cfRule type="expression" dxfId="30" priority="67">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" dxfId="144" priority="62">
+    <cfRule type="expression" dxfId="29" priority="65">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:D50">
-    <cfRule type="expression" dxfId="143" priority="61">
+    <cfRule type="expression" dxfId="28" priority="64">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:D52">
-    <cfRule type="expression" dxfId="142" priority="60">
+    <cfRule type="expression" dxfId="27" priority="63">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:B26 A29:B29 A22:B22">
-    <cfRule type="expression" dxfId="141" priority="59">
+    <cfRule type="expression" dxfId="26" priority="62">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="140" priority="57">
+    <cfRule type="expression" dxfId="25" priority="60">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31">
-    <cfRule type="expression" dxfId="139" priority="58">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:B23">
-    <cfRule type="expression" dxfId="138" priority="56">
+    <cfRule type="expression" dxfId="23" priority="59">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28">
-    <cfRule type="expression" dxfId="137" priority="55">
+    <cfRule type="expression" dxfId="22" priority="58">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30">
-    <cfRule type="expression" dxfId="136" priority="54">
+    <cfRule type="expression" dxfId="21" priority="57">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B37 A40:B40 A33:B33">
-    <cfRule type="expression" dxfId="135" priority="53">
+    <cfRule type="expression" dxfId="20" priority="56">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B38">
-    <cfRule type="expression" dxfId="134" priority="51">
+    <cfRule type="expression" dxfId="19" priority="54">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42:B42">
-    <cfRule type="expression" dxfId="133" priority="52">
+    <cfRule type="expression" dxfId="18" priority="55">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B34">
-    <cfRule type="expression" dxfId="132" priority="50">
+    <cfRule type="expression" dxfId="17" priority="53">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32">
-    <cfRule type="expression" dxfId="131" priority="49">
+    <cfRule type="expression" dxfId="16" priority="52">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39">
-    <cfRule type="expression" dxfId="130" priority="48">
+    <cfRule type="expression" dxfId="15" priority="51">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:B41">
-    <cfRule type="expression" dxfId="129" priority="47">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:B48 A51:B51 A44:B44">
-    <cfRule type="expression" dxfId="128" priority="46">
+    <cfRule type="expression" dxfId="13" priority="49">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="127" priority="44">
+    <cfRule type="expression" dxfId="12" priority="47">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:B53">
-    <cfRule type="expression" dxfId="126" priority="45">
+    <cfRule type="expression" dxfId="11" priority="48">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:B45">
-    <cfRule type="expression" dxfId="125" priority="43">
+    <cfRule type="expression" dxfId="10" priority="46">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B43">
-    <cfRule type="expression" dxfId="124" priority="42">
+    <cfRule type="expression" dxfId="9" priority="45">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="123" priority="41">
+    <cfRule type="expression" dxfId="8" priority="44">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:B52">
-    <cfRule type="expression" dxfId="122" priority="40">
+    <cfRule type="expression" dxfId="7" priority="43">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:B21">
-    <cfRule type="expression" dxfId="121" priority="39">
+    <cfRule type="expression" dxfId="6" priority="42">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="expression" dxfId="5" priority="40">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:F9">
+    <cfRule type="expression" dxfId="4" priority="39">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F53">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="120" priority="37">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E9">
-    <cfRule type="expression" dxfId="119" priority="36">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E53">
-    <cfRule type="expression" dxfId="107" priority="7">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:O6" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:P6" xr:uid="{AF93CD98-D7BE-4C5E-872E-43CDD83EAE71}">
       <formula1>TEST_OUTCOME_TYPES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>